<commit_message>
Updated data excel sheet
</commit_message>
<xml_diff>
--- a/data/Job Counts.xlsx
+++ b/data/Job Counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobceles/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msw118/Library/CloudStorage/Box-Box/Jobrole Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF866C-4875-0947-AE8E-3E455C68B313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B41A0550-324A-2F4F-8E79-1C55466E5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{95F973F6-D542-954F-8744-5D8DC6F37894}"/>
+    <workbookView xWindow="1300" yWindow="7980" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{95F973F6-D542-954F-8744-5D8DC6F37894}"/>
   </bookViews>
   <sheets>
     <sheet name="Query" sheetId="1" r:id="rId1"/>
@@ -1106,6 +1106,1347 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$K$3:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4543</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5869</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5410</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7066</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4644</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4919</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-03AC-CD43-895F-030CF7D28DD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$L$3:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19878</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17907</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21965</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20558</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22727</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15958</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16751</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31245</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26330</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21548</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35939</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-03AC-CD43-895F-030CF7D28DD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$M$3:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3610</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3837</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3488</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5514</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3839</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4766</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3980</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2871</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-03AC-CD43-895F-030CF7D28DD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$N$3:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7910</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7593</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7850</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7349</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10453</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9598</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11933</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8533</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-03AC-CD43-895F-030CF7D28DD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="672782784"/>
+        <c:axId val="672244080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="672782784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672244080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="672244080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672782784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B06C10D0-3A43-7EA6-9532-5F661CCC9ECF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13595,10 +14936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{198FEC55-2821-C04A-8F3C-DCE2F8526267}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13611,7 +14952,7 @@
     <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:14">
       <c r="A1" s="7">
         <v>2010</v>
       </c>
@@ -13625,7 +14966,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
@@ -13644,8 +14985,20 @@
       <c r="H2" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>15</v>
+      </c>
+      <c r="M2">
+        <v>27</v>
+      </c>
+      <c r="N2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3">
         <v>13</v>
       </c>
@@ -13664,8 +15017,23 @@
       <c r="H3" s="3">
         <v>5888</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3">
+        <v>2010</v>
+      </c>
+      <c r="K3" s="3">
+        <v>5106</v>
+      </c>
+      <c r="L3" s="3">
+        <v>19878</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3610</v>
+      </c>
+      <c r="N3" s="3">
+        <v>7910</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="3">
         <v>15</v>
       </c>
@@ -13684,8 +15052,23 @@
       <c r="H4" s="3">
         <v>21548</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4">
+        <v>2011</v>
+      </c>
+      <c r="K4" s="3">
+        <v>4543</v>
+      </c>
+      <c r="L4" s="3">
+        <v>17907</v>
+      </c>
+      <c r="M4" s="3">
+        <v>3666</v>
+      </c>
+      <c r="N4" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3">
         <v>27</v>
       </c>
@@ -13704,8 +15087,23 @@
       <c r="H5" s="3">
         <v>2871</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5">
+        <v>2012</v>
+      </c>
+      <c r="K5" s="3">
+        <v>5138</v>
+      </c>
+      <c r="L5" s="3">
+        <v>21965</v>
+      </c>
+      <c r="M5" s="3">
+        <v>3788</v>
+      </c>
+      <c r="N5" s="3">
+        <v>7593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3">
         <v>41</v>
       </c>
@@ -13724,13 +15122,43 @@
       <c r="H6" s="3">
         <v>6105</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="18">
+      <c r="J6">
+        <v>2013</v>
+      </c>
+      <c r="K6" s="3">
+        <v>5869</v>
+      </c>
+      <c r="L6" s="3">
+        <v>23395</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3837</v>
+      </c>
+      <c r="N6" s="3">
+        <v>7850</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18">
       <c r="A7" s="4"/>
       <c r="D7" s="4"/>
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7">
+        <v>2014</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5410</v>
+      </c>
+      <c r="L7" s="3">
+        <v>20558</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3488</v>
+      </c>
+      <c r="N7" s="3">
+        <v>6859</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="5">
         <v>2011</v>
       </c>
@@ -13743,8 +15171,23 @@
         <v>2021</v>
       </c>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8">
+        <v>2015</v>
+      </c>
+      <c r="K8" s="3">
+        <v>7066</v>
+      </c>
+      <c r="L8" s="3">
+        <v>22727</v>
+      </c>
+      <c r="M8" s="3">
+        <v>5514</v>
+      </c>
+      <c r="N8" s="3">
+        <v>11806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>166</v>
       </c>
@@ -13763,8 +15206,23 @@
       <c r="H9" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9">
+        <v>2016</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4644</v>
+      </c>
+      <c r="L9" s="3">
+        <v>15958</v>
+      </c>
+      <c r="M9" s="3">
+        <v>3995</v>
+      </c>
+      <c r="N9" s="3">
+        <v>7349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3">
         <v>13</v>
       </c>
@@ -13783,8 +15241,23 @@
       <c r="H10" s="3">
         <v>10665</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10">
+        <v>2017</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4919</v>
+      </c>
+      <c r="L10" s="3">
+        <v>16751</v>
+      </c>
+      <c r="M10" s="3">
+        <v>3839</v>
+      </c>
+      <c r="N10" s="3">
+        <v>10453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="3">
         <v>15</v>
       </c>
@@ -13803,8 +15276,23 @@
       <c r="H11" s="3">
         <v>35939</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="J11">
+        <v>2018</v>
+      </c>
+      <c r="K11" s="3">
+        <v>8443</v>
+      </c>
+      <c r="L11" s="3">
+        <v>31245</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4766</v>
+      </c>
+      <c r="N11" s="3">
+        <v>9598</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3">
         <v>27</v>
       </c>
@@ -13823,8 +15311,23 @@
       <c r="H12" s="3">
         <v>5184</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="J12">
+        <v>2019</v>
+      </c>
+      <c r="K12" s="3">
+        <v>7991</v>
+      </c>
+      <c r="L12" s="3">
+        <v>26330</v>
+      </c>
+      <c r="M12" s="3">
+        <v>3980</v>
+      </c>
+      <c r="N12" s="3">
+        <v>11933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="3">
         <v>41</v>
       </c>
@@ -13843,12 +15346,42 @@
       <c r="H13" s="3">
         <v>8533</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="18">
+      <c r="J13">
+        <v>2020</v>
+      </c>
+      <c r="K13" s="3">
+        <v>5888</v>
+      </c>
+      <c r="L13" s="3">
+        <v>21548</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2871</v>
+      </c>
+      <c r="N13" s="3">
+        <v>6105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18">
       <c r="A14" s="4"/>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="J14">
+        <v>2021</v>
+      </c>
+      <c r="K14" s="3">
+        <v>10665</v>
+      </c>
+      <c r="L14" s="3">
+        <v>35939</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5184</v>
+      </c>
+      <c r="N14" s="3">
+        <v>8533</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="5">
         <v>2012</v>
       </c>
@@ -13858,7 +15391,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>166</v>
       </c>
@@ -14102,11 +15635,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="A29:B29"/>
@@ -14114,8 +15642,14 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>